<commit_message>
MACella 2 papers added
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monicacella/Desktop/QLSC600D2_2025_M5A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE88D6F2-96DD-194A-B87F-988495D871C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43ACDD0-A87B-DA4D-8DD9-A51E51E478DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="500" windowWidth="27920" windowHeight="17500" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
+    <workbookView xWindow="2960" yWindow="620" windowWidth="24700" windowHeight="14900" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Deadlines" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Link to article</t>
   </si>
@@ -118,13 +118,74 @@
   </si>
   <si>
     <t>Evaluation scoring tailored to each column criterium?</t>
+  </si>
+  <si>
+    <t>Cartography of opportunistic pathogens and antibiotic resistance genes in a tertiary hospital environment</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41591-020-0894-4</t>
+  </si>
+  <si>
+    <t>Monica Cella</t>
+  </si>
+  <si>
+    <t>Linking the resistome and plasmidome to the microbiome</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41396-019-0446-4</t>
+  </si>
+  <si>
+    <t>N/A (?)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="3" tint="0.499984740745262"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Add column for Journal name? How good is the literature review in the introduction? "Quality of experimental design" and "Description of methods" kind of overlap - merge? I think we should remove any mention of cost of equipment, that is a barrier to equity in research not reproducibility/replicability (discussion for another day).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">This paper is difficult to replicate because it is location and time specific (environmental surveillance) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">How far-reaching are conclusions and is evidence provided to support these statements? Are too many assumptions made to reach a conclusion? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>This particular paper is difficult to replicate because it is location and time specific (and poorly designed)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,6 +242,41 @@
       <u/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="3" tint="0.499984740745262"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="3" tint="0.499984740745262"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -321,10 +417,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -362,6 +459,42 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -371,29 +504,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -803,14 +916,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
@@ -821,7 +934,7 @@
     <col min="10" max="10" width="14.1640625" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="14.1640625" customWidth="1"/>
-    <col min="13" max="13" width="49.5" customWidth="1"/>
+    <col min="13" max="13" width="101.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -838,29 +951,29 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="17" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="18"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -878,21 +991,21 @@
       <c r="J3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
@@ -908,44 +1021,92 @@
       <c r="J4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="26"/>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="28"/>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="18">
+        <v>2020</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="18">
+        <v>5</v>
+      </c>
+      <c r="G5" s="18">
+        <v>4</v>
+      </c>
+      <c r="H5" s="18">
+        <v>5</v>
+      </c>
+      <c r="I5" s="18">
+        <v>4</v>
+      </c>
+      <c r="J5" s="18">
+        <v>5</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="18">
+        <v>5</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f>A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2019</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="18">
+        <v>4</v>
+      </c>
+      <c r="G6" s="18">
+        <v>1</v>
+      </c>
+      <c r="H6" s="18">
+        <v>1</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0</v>
+      </c>
+      <c r="J6" s="18">
+        <v>3</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="18">
+        <v>1</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -955,7 +1116,9 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -973,7 +1136,9 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -991,7 +1156,9 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1814,16 +1981,19 @@
     <row r="55" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{76023512-4294-824B-9C48-0092BD200719}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Megan: Testing if I can push changes using the github desktop app.
Claimed 5 rows as "Megan Ng"
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dandantan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganng/Documents/GitHub/QLSC600D2_2025_M5A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B598DB5-7172-CB4E-8277-4A7601830997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DEB719-7CAE-9244-B275-4CFD00EF2448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Link to article</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>The code and data can be found in the original paper, the method is described clearly. The results obtained from the data are slightly different from the paper</t>
+  </si>
+  <si>
+    <t>Megan Ng</t>
   </si>
 </sst>
 </file>
@@ -940,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,7 +1347,9 @@
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1362,7 +1367,9 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1380,7 +1387,9 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1398,7 +1407,9 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>

</xml_diff>

<commit_message>
Megan: Fixing file name typo
</commit_message>
<xml_diff>
--- a/Cols_draft_M5.xlsx
+++ b/Cols_draft_M5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganng/Documents/GitHub/QLSC600D2_2025_M5A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DEB719-7CAE-9244-B275-4CFD00EF2448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B48DB5-F3BA-FC46-BF3C-9E3857853611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{36676770-CB25-F949-8228-BA136C80F5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Deadlines" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Link to article</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Megan Ng</t>
+  </si>
+  <si>
+    <t>Organizing principles of astrocytic nanoarchitecture in the mouse cerebral cortex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubmed.ncbi.nlm.nih.gov/36805126/ </t>
   </si>
 </sst>
 </file>
@@ -943,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037553EA-793E-E147-BDF6-0B4A3FE59E4A}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1212,7 @@
       <c r="C10" s="18">
         <v>2022</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="18" t="s">
@@ -1248,7 +1254,7 @@
       <c r="C11" s="22">
         <v>2021</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="18" t="s">
@@ -1284,9 +1290,15 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2023</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="E12" s="18" t="s">
         <v>35</v>
       </c>
@@ -2082,6 +2094,9 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{76023512-4294-824B-9C48-0092BD200719}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{F5278718-A4B4-4240-985E-B0483DC8FE28}"/>
+    <hyperlink ref="D10" r:id="rId3" xr:uid="{D9D5E1C5-2E77-904A-AA9E-B48D428046B2}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{05674F12-7BCD-F047-B51E-2A47BBB4405F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>